<commit_message>
get Rules from memory or from TSmatchINFO.xlsx/Rules
</commit_message>
<xml_diff>
--- a/exceldesign/База комплектующих/СтальхолдингM.xlsx
+++ b/exceldesign/База комплектующих/СтальхолдингM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pavel_Khrapkin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProgramData\Tekla Structures\2016\environments\common\exceldesign\База комплектующих\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,8 +13,9 @@
   </bookViews>
   <sheets>
     <sheet name="Уголок равнопол." sheetId="1" r:id="rId1"/>
-    <sheet name="Полоса" sheetId="2" r:id="rId2"/>
-    <sheet name="Лист г.к" sheetId="3" r:id="rId3"/>
+    <sheet name="Уголок неравнополочный" sheetId="4" r:id="rId2"/>
+    <sheet name="Полоса" sheetId="2" r:id="rId3"/>
+    <sheet name="Лист г.к" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="370">
   <si>
     <t>Наименование</t>
   </si>
@@ -1079,18 +1080,76 @@
   </si>
   <si>
     <t>PL12x100</t>
+  </si>
+  <si>
+    <t>Цена руб./тн</t>
+  </si>
+  <si>
+    <t>Уголок 63x40x5</t>
+  </si>
+  <si>
+    <t>41 990</t>
+  </si>
+  <si>
+    <t>Уголок 63x40x6</t>
+  </si>
+  <si>
+    <t>39 990</t>
+  </si>
+  <si>
+    <t>Уголок 75x50x5</t>
+  </si>
+  <si>
+    <t>Уголок 75x50x6</t>
+  </si>
+  <si>
+    <t>Уголок 100x63x6</t>
+  </si>
+  <si>
+    <t>37 990</t>
+  </si>
+  <si>
+    <t>Уголок 100x63x8</t>
+  </si>
+  <si>
+    <t>37 790</t>
+  </si>
+  <si>
+    <t>Уголок 125x80x10</t>
+  </si>
+  <si>
+    <t>48 990</t>
+  </si>
+  <si>
+    <t>Уголок 160x100x10</t>
+  </si>
+  <si>
+    <t>49 000</t>
+  </si>
+  <si>
+    <t>40 690</t>
+  </si>
+  <si>
+    <t>СТАЛЬХОЛДИНГ</t>
+  </si>
+  <si>
+    <t>Уголок неравнополочный</t>
+  </si>
+  <si>
+    <t>ГОСТ 8510-93/86</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0\ _₽_-;\-* #,##0\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1129,8 +1188,51 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF373636"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1143,8 +1245,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF9F9F9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3F3F3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1170,12 +1302,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1226,8 +1374,46 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="5" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Финансовый" xfId="1" builtinId="3"/>
   </cellStyles>
@@ -1242,6 +1428,121 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1114425</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>157809</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Рисунок 2" descr=" » Уголок "/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="647700" y="38100"/>
+          <a:ext cx="1143000" cy="700734"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1085850</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>69288</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Рисунок 4" descr="Металлический уголок"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5572125" y="0"/>
+          <a:ext cx="1085850" cy="840813"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1544,7 +1845,7 @@
   <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2669,9 +2970,292 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18">
+        <v>42889</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>351</v>
+      </c>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="30" t="s">
+        <v>229</v>
+      </c>
+      <c r="B7" s="29" t="str">
+        <f>C7</f>
+        <v>Уголок 63x40x5</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>352</v>
+      </c>
+      <c r="D7" s="22">
+        <v>63</v>
+      </c>
+      <c r="E7" s="22">
+        <v>12000</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
+        <v>229</v>
+      </c>
+      <c r="B8" s="29" t="str">
+        <f t="shared" ref="B8:B16" si="0">C8</f>
+        <v>Уголок 63x40x6</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>354</v>
+      </c>
+      <c r="D8" s="24">
+        <v>63</v>
+      </c>
+      <c r="E8" s="24">
+        <v>12000</v>
+      </c>
+      <c r="F8" s="24" t="s">
+        <v>355</v>
+      </c>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="30" t="s">
+        <v>229</v>
+      </c>
+      <c r="B9" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>Уголок 75x50x5</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>356</v>
+      </c>
+      <c r="D9" s="22">
+        <v>75</v>
+      </c>
+      <c r="E9" s="22">
+        <v>12000</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="30" t="s">
+        <v>229</v>
+      </c>
+      <c r="B10" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>Уголок 75x50x6</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="D10" s="24">
+        <v>75</v>
+      </c>
+      <c r="E10" s="24">
+        <v>12000</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="30" t="s">
+        <v>229</v>
+      </c>
+      <c r="B11" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>Уголок 100x63x6</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>358</v>
+      </c>
+      <c r="D11" s="22">
+        <v>100</v>
+      </c>
+      <c r="E11" s="22">
+        <v>12000</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>359</v>
+      </c>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="30" t="s">
+        <v>229</v>
+      </c>
+      <c r="B12" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>Уголок 100x63x8</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>360</v>
+      </c>
+      <c r="D12" s="24">
+        <v>100</v>
+      </c>
+      <c r="E12" s="24">
+        <v>12000</v>
+      </c>
+      <c r="F12" s="24" t="s">
+        <v>361</v>
+      </c>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="30" t="s">
+        <v>229</v>
+      </c>
+      <c r="B13" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>Уголок 125x80x10</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>362</v>
+      </c>
+      <c r="D13" s="26">
+        <v>125</v>
+      </c>
+      <c r="E13" s="26">
+        <v>12000</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>363</v>
+      </c>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="30" t="s">
+        <v>229</v>
+      </c>
+      <c r="B14" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>Уголок 160x100x10</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>364</v>
+      </c>
+      <c r="D14" s="24">
+        <v>160</v>
+      </c>
+      <c r="E14" s="24">
+        <v>12000</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>365</v>
+      </c>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="30" t="s">
+        <v>229</v>
+      </c>
+      <c r="B15" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>Уголок 160x100x10</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>364</v>
+      </c>
+      <c r="D15" s="22">
+        <v>160</v>
+      </c>
+      <c r="E15" s="22">
+        <v>9000</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>365</v>
+      </c>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="30" t="s">
+        <v>229</v>
+      </c>
+      <c r="B16" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>Уголок 160x100x10</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>364</v>
+      </c>
+      <c r="D16" s="24">
+        <v>160</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="24" t="s">
+        <v>366</v>
+      </c>
+      <c r="G16" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
@@ -4585,11 +5169,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>